<commit_message>
✨ feat: Updated template_excel_data_guru.xlsx file
</commit_message>
<xml_diff>
--- a/public/assets/template/template_excel_data_guru.xlsx
+++ b/public/assets/template/template_excel_data_guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\febry\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0336147F-CE36-45CC-9394-1424B2264738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ECF5AC0-F92E-455F-847C-8D9E915A0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,247 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Febry San</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B4D099A0-8131-462A-B477-8B7AE7158355}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Berisi No Urut seperti 1, 2, 3, dst</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{28B1A3E4-44E1-4481-ACBC-64ACE35F8FF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Berisi nama Guru tanpa gelar
+Contoh I Made Mudi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2F7EDE74-7614-4EB0-B1A3-219282A62CB5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jenis Kelamin berisi 
+L / P</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EE8FB76A-54CE-4104-8A38-3D21E32B6AA1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tempat Lahir 
+Contoh : Singaraja</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{01A187EF-5ADD-4200-9AE7-EA8E584D2111}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tanggal lahir format yyyy-mm-dd
+Contoh : 1989-12-31</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C20662AD-4035-4C79-ABD4-27497D371D2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NIP
+Contoh : 198609262015051001</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{8E840EC9-CD5B-480F-A6C2-80A231499BB3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status Kepegawaian
+Contoh : Tenaga Honorer/PNS/PPPK</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{14FEB8B6-E565-4D5F-AC22-410D57DC7E0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mengajar
+Contoh : 
+Pendidikan Agama dan Budi Pekerti
+Pendidikan Pancasila
+Bahasa Indonesia
+Matematika
+Ilmu Pengetahuan Alam
+Pendidikan Jasmani, Olahraga, dan Kesehatan PJOK
+Agama Hindu
+Bimbingan dan Konseling
+Bahasa Bali</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{67CF1C9C-C162-4757-8679-22BE8344BC6A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gelar Depan
+Contoh : dr, Ir</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{E3FC33FB-5C90-481C-8C9E-C4A516CCBCC1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gelar Belakang
+Contoh L M.Pd, S.Pd</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{6619F145-BBE0-458A-84E4-6DB008E6CF84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jenjang Terakhr
+Contoh : S1, S2, S3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{17AA3EBB-E139-4187-BB5F-16E0216920EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jurusan/Prodi
+Contoh : PGSD, Matematika, Agama</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{63442AC3-C0EC-4498-919D-8BD1DCDA0B1A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD
+2002-03-03</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{0D2FD983-FEB2-4778-B3D9-DBF265FA9671}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD
+2002-03-03</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{7FF98195-9FB2-436D-B94B-3BF9F9A8D4A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 = Iya
+0 = Tidak</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
@@ -175,11 +416,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,6 +481,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,11 +773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,5 +934,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>